<commit_message>
Cleaned OS6 notebook for public release
</commit_message>
<xml_diff>
--- a/docs/source/notebooks/notebook_descriptions.xlsx
+++ b/docs/source/notebooks/notebook_descriptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrizzo/IFS/crispy/docs/source/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0764CEDE-633C-5040-9DBD-03A32D6ECC9B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C53EB1C6-0C70-9F43-BD18-234139392AF5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-73800" yWindow="4540" windowWidth="28040" windowHeight="17440" xr2:uid="{47771A9F-C764-6543-9188-30509CA9D154}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="107">
   <si>
     <t>Notebook descriptions</t>
   </si>
@@ -340,6 +340,12 @@
   </si>
   <si>
     <t>Creates input files for OS6 two-roll configuration</t>
+  </si>
+  <si>
+    <t>Cleaned_OS6</t>
+  </si>
+  <si>
+    <t>Cleaned version of the OS6 HLC notebook for distribution</t>
   </si>
 </sst>
 </file>
@@ -459,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -506,6 +512,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -827,10 +836,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA51E57F-59B1-8041-9F2D-BF3E2331004A}">
-  <dimension ref="A3:C57"/>
+  <dimension ref="A3:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -895,383 +904,383 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:3" s="4" customFormat="1">
+      <c r="A12" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3" t="s">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="9" customFormat="1">
-      <c r="A13" s="10" t="s">
+    <row r="14" spans="1:3" s="9" customFormat="1">
+      <c r="A14" s="10" t="s">
         <v>10</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="9" customFormat="1" ht="32">
-      <c r="A14" s="10" t="s">
-        <v>12</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>101</v>
       </c>
       <c r="C14" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="9" customFormat="1" ht="32">
+      <c r="A15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="12" customFormat="1">
-      <c r="A15" s="11" t="s">
+    <row r="16" spans="1:3" s="12" customFormat="1">
+      <c r="A16" s="11" t="s">
         <v>103</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" s="12" customFormat="1" ht="32">
-      <c r="A16" s="11" t="s">
-        <v>14</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>102</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="12" customFormat="1">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="12" customFormat="1" ht="32">
       <c r="A17" s="11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>102</v>
       </c>
       <c r="C17" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="12" customFormat="1">
+      <c r="A18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="14" customFormat="1">
-      <c r="A18" s="13" t="s">
+    <row r="19" spans="1:3" s="14" customFormat="1">
+      <c r="A19" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B19" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C19" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="5" customFormat="1" ht="32">
-      <c r="A19" s="7" t="s">
+    <row r="20" spans="1:3" s="5" customFormat="1" ht="32">
+      <c r="A20" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" s="5" customFormat="1">
-      <c r="A20" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" s="5" customFormat="1">
+      <c r="A21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="12" customFormat="1">
-      <c r="A21" s="12" t="s">
+    <row r="22" spans="1:3" s="12" customFormat="1">
+      <c r="A22" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B22" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C22" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:3">
+      <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="9" customFormat="1">
-      <c r="A23" s="9" t="s">
+    <row r="24" spans="1:3" s="9" customFormat="1">
+      <c r="A24" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B24" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C24" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="4" customFormat="1">
-      <c r="A24" s="4" t="s">
+    <row r="25" spans="1:3" s="4" customFormat="1">
+      <c r="A25" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" s="9" customFormat="1">
-      <c r="A25" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="9" customFormat="1">
       <c r="A26" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>101</v>
       </c>
       <c r="C26" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="9" customFormat="1">
+      <c r="A27" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="5" customFormat="1">
-      <c r="A27" s="5" t="s">
+    <row r="28" spans="1:3" s="5" customFormat="1">
+      <c r="A28" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B28" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C28" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="8" customFormat="1" ht="32">
-      <c r="A28" s="8" t="s">
+    <row r="29" spans="1:3" s="8" customFormat="1" ht="32">
+      <c r="A29" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B29" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C29" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="9" customFormat="1">
-      <c r="A29" s="9" t="s">
+    <row r="30" spans="1:3" s="9" customFormat="1">
+      <c r="A30" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B30" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C30" s="9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="6" customFormat="1">
-      <c r="A30" s="6" t="s">
+    <row r="31" spans="1:3" s="6" customFormat="1">
+      <c r="A31" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B31" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C31" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="9" customFormat="1" ht="32">
-      <c r="A31" s="9" t="s">
+    <row r="32" spans="1:3" s="9" customFormat="1" ht="32">
+      <c r="A32" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B32" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C32" s="9" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" s="4" customFormat="1">
-      <c r="A32" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="4" customFormat="1">
       <c r="A33" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>97</v>
       </c>
       <c r="C33" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="4" customFormat="1">
+      <c r="A34" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>100</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>100</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>100</v>
       </c>
       <c r="C37" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="9" customFormat="1">
-      <c r="A38" s="9" t="s">
+    <row r="39" spans="1:3" s="9" customFormat="1">
+      <c r="A39" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B39" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C39" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A39" s="4" t="s">
+    <row r="40" spans="1:3" s="4" customFormat="1" ht="15" customHeight="1">
+      <c r="A40" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" s="4" customFormat="1">
-      <c r="A40" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>97</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:3" s="4" customFormat="1">
       <c r="A41" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>97</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:3" s="4" customFormat="1">
       <c r="A42" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>97</v>
       </c>
       <c r="C42" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" s="4" customFormat="1">
+      <c r="A43" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="9" customFormat="1">
-      <c r="A45" s="9" t="s">
+    <row r="45" spans="1:3">
+      <c r="A45" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" s="9" customFormat="1">
+      <c r="A46" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B46" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C45" s="9" t="s">
+      <c r="C46" s="9" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" s="4" customFormat="1">
-      <c r="A46" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="47" spans="1:3" s="4" customFormat="1">
       <c r="A47" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>97</v>
@@ -1280,64 +1289,64 @@
         <v>74</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="5" customFormat="1">
-      <c r="A48" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>77</v>
+    <row r="48" spans="1:3" s="4" customFormat="1">
+      <c r="A48" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:3" s="5" customFormat="1">
       <c r="A49" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>98</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="50" spans="1:3" s="5" customFormat="1">
       <c r="A50" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>98</v>
       </c>
       <c r="C50" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" s="5" customFormat="1">
+      <c r="A51" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C51" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="51" spans="1:3" s="6" customFormat="1">
-      <c r="A51" s="6" t="s">
+    <row r="52" spans="1:3" s="6" customFormat="1">
+      <c r="A52" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B52" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C51" s="6" t="s">
+      <c r="C52" s="6" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" s="14" customFormat="1">
-      <c r="A52" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B52" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="C52" s="14" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:3" s="14" customFormat="1">
       <c r="A53" s="14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B53" s="14" t="s">
         <v>101</v>
@@ -1346,47 +1355,58 @@
         <v>85</v>
       </c>
     </row>
-    <row r="54" spans="1:3" s="12" customFormat="1">
-      <c r="A54" s="12" t="s">
+    <row r="54" spans="1:3" s="14" customFormat="1">
+      <c r="A54" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" s="12" customFormat="1">
+      <c r="A55" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="B54" s="11" t="s">
+      <c r="B55" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="C54" s="12" t="s">
+      <c r="C55" s="12" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" s="8" customFormat="1">
-      <c r="A55" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="56" spans="1:3" s="8" customFormat="1">
       <c r="A56" s="8" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>96</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="57" spans="1:3" s="8" customFormat="1">
       <c r="A57" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B57" s="8" t="s">
         <v>96</v>
       </c>
       <c r="C57" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" s="8" customFormat="1">
+      <c r="A58" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C58" s="8" t="s">
         <v>94</v>
       </c>
     </row>

</xml_diff>